<commit_message>
SSDM-13163 Added the description attribute to exports. Removed background color checking from assertions because the tests with this check will be difficult to maintain in different OSs.
</commit_message>
<xml_diff>
--- a/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-filtered-properties.xlsx
+++ b/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-filtered-properties.xlsx
@@ -230,36 +230,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -299,27 +297,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" s="6" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -332,6 +328,7 @@
       <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">

</xml_diff>